<commit_message>
Program writes to a file.
</commit_message>
<xml_diff>
--- a/DyeListGenerator.Test/Resources/MasterDyeList.xlsx
+++ b/DyeListGenerator.Test/Resources/MasterDyeList.xlsx
@@ -1,7 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr date1904="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
@@ -95,13 +94,13 @@
     <t>Mini BFL DK</t>
   </si>
   <si>
-    <t>19th! DOTS</t>
+    <t>19TH!</t>
   </si>
   <si>
     <t>1R</t>
   </si>
   <si>
-    <t>6 of Everything</t>
+    <t>6 OF EVERYTHING</t>
   </si>
   <si>
     <t>5T</t>
@@ -113,31 +112,31 @@
     <t>E5</t>
   </si>
   <si>
-    <t xml:space="preserve">Absolute Magenta </t>
+    <t>ABSOLUTE MAGENTA</t>
   </si>
   <si>
     <t>O4</t>
   </si>
   <si>
-    <t>after hours</t>
+    <t>AFTER HOURS</t>
   </si>
   <si>
     <t>3B</t>
   </si>
   <si>
-    <t>Alive</t>
+    <t>ALIVE</t>
   </si>
   <si>
     <t>3G</t>
   </si>
   <si>
-    <t>All American Hen</t>
+    <t>ALL AMERICAN HEN</t>
   </si>
   <si>
     <t>3R</t>
   </si>
   <si>
-    <t>Amber Glass</t>
+    <t>AMBER GLASS</t>
   </si>
   <si>
     <t>Z1</t>
@@ -149,7 +148,7 @@
     <t>E3</t>
   </si>
   <si>
-    <t>Amethyst Ink</t>
+    <t>AMETHYST INK</t>
   </si>
   <si>
     <t>H4</t>
@@ -161,52 +160,52 @@
     <t>E1</t>
   </si>
   <si>
-    <t>Angelica</t>
+    <t>ANGELICA</t>
   </si>
   <si>
     <t>E2</t>
   </si>
   <si>
-    <t>angels landing</t>
+    <t>ANGEL’S LANDING</t>
   </si>
   <si>
     <t>F2</t>
   </si>
   <si>
-    <t>anything goes</t>
-  </si>
-  <si>
-    <t>Apathy</t>
+    <t>ANYTHING GOES</t>
+  </si>
+  <si>
+    <t>APATHY</t>
   </si>
   <si>
     <t>H1</t>
   </si>
   <si>
-    <t xml:space="preserve">Aqua Jet </t>
+    <t>AQUA JET</t>
   </si>
   <si>
     <t>H3</t>
   </si>
   <si>
-    <t>As a Bird</t>
+    <t>AS A BIRD</t>
   </si>
   <si>
     <t>Z3</t>
   </si>
   <si>
-    <t>Atomic Blue</t>
+    <t>ATOMIC BLUE</t>
   </si>
   <si>
     <t>Z4</t>
   </si>
   <si>
-    <t>Awesome, Wow</t>
+    <t>AWESOME! WOW!</t>
   </si>
   <si>
     <t>E0</t>
   </si>
   <si>
-    <t xml:space="preserve">Azure cove </t>
+    <t>AZURE COVE</t>
   </si>
   <si>
     <t>BASALT</t>
@@ -215,19 +214,19 @@
     <t>E4</t>
   </si>
   <si>
-    <t>bedtime</t>
-  </si>
-  <si>
-    <t>Belle Epoque</t>
+    <t>BEDTIME</t>
+  </si>
+  <si>
+    <t>BELLE EPOQUE</t>
   </si>
   <si>
     <t>2R</t>
   </si>
   <si>
-    <t>below horizon</t>
-  </si>
-  <si>
-    <t>Bermuda Teal</t>
+    <t>BELOW HORIZON</t>
+  </si>
+  <si>
+    <t>BERMUDA TEAL</t>
   </si>
   <si>
     <t>Z5</t>
@@ -236,7 +235,7 @@
     <t>BITTER</t>
   </si>
   <si>
-    <t>Bitter Malaise</t>
+    <t>BITTER MALAISE</t>
   </si>
   <si>
     <t>H2</t>
@@ -245,13 +244,13 @@
     <t>BLACK &amp; WHITE</t>
   </si>
   <si>
-    <t>Black Pearl</t>
+    <t>BLACK PEARL</t>
   </si>
   <si>
     <t>Z6</t>
   </si>
   <si>
-    <t>BlancheFleur DOTS</t>
+    <t>BLANCHEFLEUR</t>
   </si>
   <si>
     <t>1T</t>
@@ -260,19 +259,19 @@
     <t>BLUE FISH</t>
   </si>
   <si>
-    <t>blue lagoon</t>
-  </si>
-  <si>
-    <t>Blue Sage</t>
+    <t>BLUE LAGOON</t>
+  </si>
+  <si>
+    <t>BLUE SAGE</t>
   </si>
   <si>
     <t>O1</t>
   </si>
   <si>
-    <t>Blue Sulk</t>
-  </si>
-  <si>
-    <t>Boot Camp</t>
+    <t>BLUE SULK</t>
+  </si>
+  <si>
+    <t>BOOT CAMP</t>
   </si>
   <si>
     <t>BRILLIANT</t>
@@ -284,22 +283,22 @@
     <t>BURR</t>
   </si>
   <si>
-    <t>Cabaret</t>
-  </si>
-  <si>
-    <t>Caldera</t>
+    <t>CABARET</t>
+  </si>
+  <si>
+    <t>CALDERA</t>
   </si>
   <si>
     <t>3N</t>
   </si>
   <si>
-    <t>Callous Pink</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Candy love </t>
-  </si>
-  <si>
-    <t>Carmen miranda</t>
+    <t>CALLOUS PINK</t>
+  </si>
+  <si>
+    <t>CANDY LOVE</t>
+  </si>
+  <si>
+    <t>CARMEN MIRANDA</t>
   </si>
   <si>
     <t>O2</t>
@@ -308,49 +307,49 @@
     <t>CAROLINA</t>
   </si>
   <si>
-    <t>carousel</t>
-  </si>
-  <si>
-    <t>Catching Stars</t>
-  </si>
-  <si>
-    <t>cedar creek</t>
+    <t>CAROUSEL</t>
+  </si>
+  <si>
+    <t>CATCHING STARS</t>
+  </si>
+  <si>
+    <t>CEDAR CREEK</t>
   </si>
   <si>
     <t>Z2</t>
   </si>
   <si>
-    <t>Charcoal Prismatic</t>
+    <t>CHARCOAL PRISMATIC</t>
   </si>
   <si>
     <t>5R</t>
   </si>
   <si>
-    <t>Charged Cherry</t>
-  </si>
-  <si>
-    <t>Charli’s Au Lait</t>
-  </si>
-  <si>
-    <t>Chesley</t>
+    <t>CHARGED CHERRY</t>
+  </si>
+  <si>
+    <t>CHARLI AU LAIT</t>
+  </si>
+  <si>
+    <t>CHESLEY</t>
   </si>
   <si>
     <t>CHILI</t>
   </si>
   <si>
-    <t>Chocolate Night</t>
-  </si>
-  <si>
-    <t>Cinnamon Girl</t>
-  </si>
-  <si>
-    <t>cities, tower &amp; bridges</t>
+    <t>CHOCOLATE NIGHT</t>
+  </si>
+  <si>
+    <t>CINNAMON GIRL</t>
+  </si>
+  <si>
+    <t>CITIES TOWERS &amp; BRIDGES</t>
   </si>
   <si>
     <t>5P</t>
   </si>
   <si>
-    <t>Cloud To ground</t>
+    <t>CLOUD TO GROUND</t>
   </si>
   <si>
     <t>5Y</t>
@@ -371,13 +370,13 @@
     <t>CRISP</t>
   </si>
   <si>
-    <t>Crying Dove</t>
+    <t>CRYING DOVE</t>
   </si>
   <si>
     <t>CRYSTAL STORM</t>
   </si>
   <si>
-    <t>Damp Pillow</t>
+    <t>DAMP PILLOW</t>
   </si>
   <si>
     <t>DARK CURRENT</t>
@@ -386,22 +385,22 @@
     <t>DAYLILLY</t>
   </si>
   <si>
-    <t>Deep Regret</t>
-  </si>
-  <si>
-    <t>deep seaflower</t>
-  </si>
-  <si>
-    <t>Desert city wattage</t>
+    <t>DEEP REGRET</t>
+  </si>
+  <si>
+    <t>DEEP SEAFLOWER</t>
+  </si>
+  <si>
+    <t>DESERT CITY WATTAGE</t>
   </si>
   <si>
     <t>3Y</t>
   </si>
   <si>
-    <t xml:space="preserve">Desert oasis </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Devils garden </t>
+    <t>DESERT OASIS</t>
+  </si>
+  <si>
+    <t>DEVIL’S GARDEN</t>
   </si>
   <si>
     <t>F3</t>
@@ -410,25 +409,25 @@
     <t>DIVE</t>
   </si>
   <si>
-    <t>divine</t>
-  </si>
-  <si>
-    <t>Do Re Me</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dream on </t>
-  </si>
-  <si>
-    <t>dreamgirls</t>
-  </si>
-  <si>
-    <t>Dune</t>
-  </si>
-  <si>
-    <t>dusk to dawn</t>
-  </si>
-  <si>
-    <t>eaten the plums</t>
+    <t>DIVINE</t>
+  </si>
+  <si>
+    <t>DO RE ME</t>
+  </si>
+  <si>
+    <t>DREAM ON!</t>
+  </si>
+  <si>
+    <t>DREAMGIRLS</t>
+  </si>
+  <si>
+    <t>DUNE</t>
+  </si>
+  <si>
+    <t>DUSK TO DAWN</t>
+  </si>
+  <si>
+    <t>EATEN THE PLUMS</t>
   </si>
   <si>
     <t>3P</t>
@@ -440,16 +439,16 @@
     <t xml:space="preserve">ELECTRIC MAUVE </t>
   </si>
   <si>
-    <t>Element 79</t>
-  </si>
-  <si>
-    <t>Eliza</t>
+    <t>ELEMENT 79</t>
+  </si>
+  <si>
+    <t>ELIZA</t>
   </si>
   <si>
     <t>ELYSIAN</t>
   </si>
   <si>
-    <t>Emerald Darkness</t>
+    <t>EMERALD DARKNESS</t>
   </si>
   <si>
     <t>H5</t>
@@ -458,46 +457,46 @@
     <t xml:space="preserve">EVENING FLAME </t>
   </si>
   <si>
-    <t>Fable  DOTS</t>
+    <t>FABLE</t>
   </si>
   <si>
     <t>1G</t>
   </si>
   <si>
-    <t>fancy</t>
-  </si>
-  <si>
-    <t>Fatal Duel</t>
-  </si>
-  <si>
-    <t>Federal Bank</t>
-  </si>
-  <si>
-    <t>Fern Slipper</t>
-  </si>
-  <si>
-    <t>Fierce Scarlet</t>
-  </si>
-  <si>
-    <t>flower drum song</t>
-  </si>
-  <si>
-    <t>Forget Me</t>
+    <t>FANCY</t>
+  </si>
+  <si>
+    <t>FATAL DUEL</t>
+  </si>
+  <si>
+    <t>FEDERAL BANK</t>
+  </si>
+  <si>
+    <t>FERN SLIPPER</t>
+  </si>
+  <si>
+    <t>FIERCE SCARLET</t>
+  </si>
+  <si>
+    <t>FLOWER DRUM SONG</t>
+  </si>
+  <si>
+    <t>FORGET ME</t>
   </si>
   <si>
     <t>FORTUNE</t>
   </si>
   <si>
-    <t>Fortune Teller</t>
+    <t>FORTUNE TELLER</t>
   </si>
   <si>
     <t>GALAXY</t>
   </si>
   <si>
-    <t xml:space="preserve">Get down greeny </t>
-  </si>
-  <si>
-    <t>GG Laurel</t>
+    <t>GET DOWN GREENY</t>
+  </si>
+  <si>
+    <t>GG LAUREL</t>
   </si>
   <si>
     <t>5G</t>
@@ -509,70 +508,70 @@
     <t>GILT</t>
   </si>
   <si>
-    <t xml:space="preserve">Goblin Valley </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gold Experience </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gold mine </t>
-  </si>
-  <si>
-    <t>good luck jade</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Green Lantern </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grey Tabby </t>
+    <t>GOBLIN VALLEY</t>
+  </si>
+  <si>
+    <t>GOLD EXPERIENCE</t>
+  </si>
+  <si>
+    <t>GOLD MINE</t>
+  </si>
+  <si>
+    <t>GOOD LUCK JADE</t>
+  </si>
+  <si>
+    <t>GREEN LANTERN</t>
+  </si>
+  <si>
+    <t>GREY TABBY</t>
   </si>
   <si>
     <t>GROW</t>
   </si>
   <si>
-    <t>Guthrie Peak</t>
-  </si>
-  <si>
-    <t>Haywire</t>
-  </si>
-  <si>
-    <t>Hear it hawaii</t>
+    <t>GUTHRIE PEAK</t>
+  </si>
+  <si>
+    <t>HAYWIRE</t>
+  </si>
+  <si>
+    <t>HEAR IT HAWAII</t>
   </si>
   <si>
     <t>HEAVENLY</t>
   </si>
   <si>
-    <t>Hello Dolly!</t>
-  </si>
-  <si>
-    <t>her beacon hand</t>
-  </si>
-  <si>
-    <t>Her Charisma</t>
+    <t>HELLO DOLLY!</t>
+  </si>
+  <si>
+    <t>HER BEACON HAND</t>
+  </si>
+  <si>
+    <t>HER CHARISMA</t>
   </si>
   <si>
     <t>HERBAL</t>
   </si>
   <si>
-    <t xml:space="preserve">Hey sunshine </t>
+    <t>HEY SUNSHINE!</t>
   </si>
   <si>
     <t>HOLLY</t>
   </si>
   <si>
-    <t xml:space="preserve">Hot air balloon </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hot pants </t>
-  </si>
-  <si>
-    <t>Humdrum</t>
-  </si>
-  <si>
-    <t>Iceland</t>
-  </si>
-  <si>
-    <t>Icy Reception</t>
+    <t>HOT AIR BALLOON</t>
+  </si>
+  <si>
+    <t>HOT PANTS</t>
+  </si>
+  <si>
+    <t>HUMDRUM</t>
+  </si>
+  <si>
+    <t>ICELAND</t>
+  </si>
+  <si>
+    <t>ICY RECEPTION</t>
   </si>
   <si>
     <t>INDIGO</t>
@@ -581,160 +580,160 @@
     <t>ISLAND</t>
   </si>
   <si>
-    <t>It’s A sparkler</t>
-  </si>
-  <si>
-    <t>Ivy Snowbell DOTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jay feather </t>
+    <t>IT’S A SPARKLER</t>
+  </si>
+  <si>
+    <t>IVY SNOWBELL</t>
+  </si>
+  <si>
+    <t>JAY FEATHER</t>
   </si>
   <si>
     <t>JEANS</t>
   </si>
   <si>
-    <t>Jessamyn</t>
+    <t>JESSAMYN</t>
   </si>
   <si>
     <t>3T</t>
   </si>
   <si>
-    <t>Jocelyn</t>
-  </si>
-  <si>
-    <t>Joshua tree</t>
-  </si>
-  <si>
-    <t>JuliEtte's Blush</t>
-  </si>
-  <si>
-    <t>just to say</t>
-  </si>
-  <si>
-    <t>K Chameleon</t>
-  </si>
-  <si>
-    <t>kiss me kate</t>
-  </si>
-  <si>
-    <t>Kyoto sunset</t>
-  </si>
-  <si>
-    <t>La luz</t>
-  </si>
-  <si>
-    <t>Lafayette</t>
-  </si>
-  <si>
-    <t>Lavender Bloom</t>
-  </si>
-  <si>
-    <t>Lay a Rose</t>
-  </si>
-  <si>
-    <t>Leaf, seed, bean</t>
-  </si>
-  <si>
-    <t>leprechaun ballet</t>
-  </si>
-  <si>
-    <t>liberation</t>
-  </si>
-  <si>
-    <t>life of the gods</t>
-  </si>
-  <si>
-    <t>lipstick lava</t>
-  </si>
-  <si>
-    <t>little green men</t>
+    <t>JOCELYN</t>
+  </si>
+  <si>
+    <t>JOSHUA TREE</t>
+  </si>
+  <si>
+    <t>JULIETTE’S BLUSH</t>
+  </si>
+  <si>
+    <t>JUST TO SAY</t>
+  </si>
+  <si>
+    <t>K. CHAMELEON</t>
+  </si>
+  <si>
+    <t>KISS ME KATE</t>
+  </si>
+  <si>
+    <t>KYOTO SUNSET</t>
+  </si>
+  <si>
+    <t>LA LUZ</t>
+  </si>
+  <si>
+    <t>LAFAYETTE</t>
+  </si>
+  <si>
+    <t>LAVENDER BLOOM</t>
+  </si>
+  <si>
+    <t>LAY A ROSE</t>
+  </si>
+  <si>
+    <t>LEAF SEED BEAN</t>
+  </si>
+  <si>
+    <t>LEPRECHAUN BALLET</t>
+  </si>
+  <si>
+    <t>LIBERATION</t>
+  </si>
+  <si>
+    <t>LIFE OF THE GODS</t>
+  </si>
+  <si>
+    <t>LIPSTICK LAVA</t>
+  </si>
+  <si>
+    <t>LITTLE GREEN MEN</t>
   </si>
   <si>
     <t>O3</t>
   </si>
   <si>
-    <t>Loose Gems</t>
-  </si>
-  <si>
-    <t>Lost in Plum</t>
+    <t>LOOSE GEMS</t>
+  </si>
+  <si>
+    <t>LOST IN PLUM</t>
   </si>
   <si>
     <t>O5</t>
   </si>
   <si>
-    <t>Magic Orchid</t>
-  </si>
-  <si>
-    <t>Malibu Sail</t>
-  </si>
-  <si>
-    <t>medieval</t>
-  </si>
-  <si>
-    <t>Melon Bomb</t>
-  </si>
-  <si>
-    <t>mercado lights</t>
-  </si>
-  <si>
-    <t>Mermaid Shoes</t>
-  </si>
-  <si>
-    <t>Mesa</t>
-  </si>
-  <si>
-    <t>Miami Red</t>
-  </si>
-  <si>
-    <t>Mild Tedium</t>
+    <t>MAGIC ORCHID</t>
+  </si>
+  <si>
+    <t>MALIBU SAIL</t>
+  </si>
+  <si>
+    <t>MEDIEVAL</t>
+  </si>
+  <si>
+    <t>MELON BOMB</t>
+  </si>
+  <si>
+    <t>MERCADO LIGHTS</t>
+  </si>
+  <si>
+    <t>MERMAID SHOES</t>
+  </si>
+  <si>
+    <t>MESA</t>
+  </si>
+  <si>
+    <t>MIAMI RED</t>
+  </si>
+  <si>
+    <t>MILD TEDIUM</t>
   </si>
   <si>
     <t>MILKY SPITE</t>
   </si>
   <si>
-    <t>mist of nyx</t>
+    <t>MIST OF NYX</t>
   </si>
   <si>
     <t>5B</t>
   </si>
   <si>
-    <t>Moccasin</t>
-  </si>
-  <si>
-    <t>Mod squad</t>
+    <t>MOCCASIN</t>
+  </si>
+  <si>
+    <t>MOD SQUAD</t>
   </si>
   <si>
     <t>MORNING GLORY</t>
   </si>
   <si>
-    <t>my fair lady</t>
-  </si>
-  <si>
-    <t>Naked Shame</t>
-  </si>
-  <si>
-    <t>Navy Zeal</t>
+    <t>MY FAIR LADY</t>
+  </si>
+  <si>
+    <t>NAKED SHAME</t>
+  </si>
+  <si>
+    <t>NAVY ZEAL</t>
   </si>
   <si>
     <t>NEBULA</t>
   </si>
   <si>
-    <t>Nighthawks</t>
-  </si>
-  <si>
-    <t>no limit</t>
-  </si>
-  <si>
-    <t>november muse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Old pueblo </t>
-  </si>
-  <si>
-    <t>Old Vine</t>
-  </si>
-  <si>
-    <t>Out Beyond</t>
+    <t>NIGHTHAWKS</t>
+  </si>
+  <si>
+    <t>NO LIMIT</t>
+  </si>
+  <si>
+    <t>NOVEMBER MUSE</t>
+  </si>
+  <si>
+    <t>OLD PUEBLO</t>
+  </si>
+  <si>
+    <t>OLD VINE</t>
+  </si>
+  <si>
+    <t>OUT BEYOND</t>
   </si>
   <si>
     <t>4R</t>
@@ -743,28 +742,28 @@
     <t>PASSION</t>
   </si>
   <si>
-    <t>Peaceful Transition</t>
-  </si>
-  <si>
-    <t>Peacock Shadow</t>
-  </si>
-  <si>
-    <t>penchant</t>
-  </si>
-  <si>
-    <t>petal shower</t>
-  </si>
-  <si>
-    <t>petrified forest</t>
-  </si>
-  <si>
-    <t>Pickle Ball</t>
-  </si>
-  <si>
-    <t>pink bean</t>
-  </si>
-  <si>
-    <t>Pinky</t>
+    <t>PEACEFUL TRANSITION</t>
+  </si>
+  <si>
+    <t>PEACOCK SHADOW</t>
+  </si>
+  <si>
+    <t>PENCHANT</t>
+  </si>
+  <si>
+    <t>PETAL SHOWER</t>
+  </si>
+  <si>
+    <t>PETRIFIED FOREST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICKLE BALL </t>
+  </si>
+  <si>
+    <t>PINK BEAN</t>
+  </si>
+  <si>
+    <t>PINKY</t>
   </si>
   <si>
     <t>PINOT</t>
@@ -773,172 +772,172 @@
     <t>PLENTY</t>
   </si>
   <si>
-    <t>Poma-Grenade</t>
+    <t>POMAGRENADE</t>
   </si>
   <si>
     <t>POPPY</t>
   </si>
   <si>
-    <t>Power Plant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prickly pear </t>
-  </si>
-  <si>
-    <t>Prince William</t>
-  </si>
-  <si>
-    <t>punky fuchsia</t>
-  </si>
-  <si>
-    <t>Purple Rain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Queen's lake </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rabbit ears </t>
+    <t>POWER PLANT</t>
+  </si>
+  <si>
+    <t>PRICKLY PEAR</t>
+  </si>
+  <si>
+    <t>PRINCE WILLIAM</t>
+  </si>
+  <si>
+    <t>PUNKY FUSCHIA</t>
+  </si>
+  <si>
+    <t>PURPLE RAIN</t>
+  </si>
+  <si>
+    <t>QUEEN’S LAKE</t>
+  </si>
+  <si>
+    <t>RABBIT EARS</t>
   </si>
   <si>
     <t>RAIN CLOUD</t>
   </si>
   <si>
-    <t>Rain on Me</t>
-  </si>
-  <si>
-    <t>Raspberry Blaze</t>
-  </si>
-  <si>
-    <t>Red Rush</t>
-  </si>
-  <si>
-    <t>Regency</t>
-  </si>
-  <si>
-    <t>relish the vote!</t>
+    <t>RAIN ON ME</t>
+  </si>
+  <si>
+    <t>RASPBERRY BLAZE</t>
+  </si>
+  <si>
+    <t>RED RUSH</t>
+  </si>
+  <si>
+    <t>REGENCY</t>
+  </si>
+  <si>
+    <t>RELISH THE VOTE!</t>
   </si>
   <si>
     <t>RETRIEVER</t>
   </si>
   <si>
-    <t>Reynolds</t>
-  </si>
-  <si>
-    <t>ring the blossom bell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rio verde </t>
-  </si>
-  <si>
-    <t>riot girls</t>
-  </si>
-  <si>
-    <t>Rochambeau</t>
-  </si>
-  <si>
-    <t>Romeo Blue</t>
-  </si>
-  <si>
-    <t>Rosalita</t>
-  </si>
-  <si>
-    <t>Rose Anguish</t>
+    <t>REYNOLDS</t>
+  </si>
+  <si>
+    <t>RING THE BLOSSOM BELL</t>
+  </si>
+  <si>
+    <t>RIO VERDE</t>
+  </si>
+  <si>
+    <t>RIOT GIRLS</t>
+  </si>
+  <si>
+    <t>ROCHAMBEAU</t>
+  </si>
+  <si>
+    <t>ROMEO BLUE</t>
+  </si>
+  <si>
+    <t>ROSALITA</t>
+  </si>
+  <si>
+    <t>ROSE ANGUISH</t>
   </si>
   <si>
     <t>ROSY</t>
   </si>
   <si>
-    <t>route 66</t>
+    <t>ROUTE 66</t>
   </si>
   <si>
     <t>SANGRIA</t>
   </si>
   <si>
-    <t>Scorched Lime</t>
-  </si>
-  <si>
-    <t>secret garden</t>
-  </si>
-  <si>
-    <t>Shadow Box</t>
-  </si>
-  <si>
-    <t>she walks in beauty</t>
-  </si>
-  <si>
-    <t>Shiny Moss</t>
-  </si>
-  <si>
-    <t>Shuyler Lake</t>
+    <t>SCORCHED LIME</t>
+  </si>
+  <si>
+    <t>SECRET GARDEN</t>
+  </si>
+  <si>
+    <t>SHADOW BOX</t>
+  </si>
+  <si>
+    <t>SHE WALKS IN BEAUTY</t>
+  </si>
+  <si>
+    <t>SHINY MOSS</t>
+  </si>
+  <si>
+    <t>SHUYLER LAKE</t>
   </si>
   <si>
     <t>SHY</t>
   </si>
   <si>
-    <t>simone and susan</t>
-  </si>
-  <si>
-    <t>singing in the rain</t>
-  </si>
-  <si>
-    <t>Skipping Stone</t>
-  </si>
-  <si>
-    <t>Skyrocket</t>
+    <t>SIMONE &amp; SUSAN</t>
+  </si>
+  <si>
+    <t>SINGING IN THE RAIN</t>
+  </si>
+  <si>
+    <t>SKIPPING STONE</t>
+  </si>
+  <si>
+    <t>SKYROCKET</t>
   </si>
   <si>
     <t>4B</t>
   </si>
   <si>
-    <t xml:space="preserve">Slammin lemon </t>
+    <t>SLAMMIN LEMON</t>
   </si>
   <si>
     <t>SLIPPERY TRAIL</t>
   </si>
   <si>
-    <t>solar glitter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sonoran sky </t>
-  </si>
-  <si>
-    <t>south pacific</t>
-  </si>
-  <si>
-    <t>spring tickle</t>
-  </si>
-  <si>
-    <t>Sprout</t>
-  </si>
-  <si>
-    <t>Starless Sky</t>
-  </si>
-  <si>
-    <t>still i rise</t>
+    <t>SOLAR GLITTER</t>
+  </si>
+  <si>
+    <t>SONORAN SKY</t>
+  </si>
+  <si>
+    <t>SOUTH PACIFIC</t>
+  </si>
+  <si>
+    <t>SPRING TICKLE</t>
+  </si>
+  <si>
+    <t>SPROUT</t>
+  </si>
+  <si>
+    <t>STARLESS SKY</t>
+  </si>
+  <si>
+    <t>STILL I RISE</t>
   </si>
   <si>
     <t>1P</t>
   </si>
   <si>
-    <t>Still Spruce</t>
-  </si>
-  <si>
-    <t>strange harvest</t>
-  </si>
-  <si>
-    <t>Straw Into Gold</t>
-  </si>
-  <si>
-    <t>Strikes Twice</t>
-  </si>
-  <si>
-    <t>String &amp; Key  DOTS</t>
+    <t>STILL SPRUCE</t>
+  </si>
+  <si>
+    <t>STRANGE HARVEST</t>
+  </si>
+  <si>
+    <t>STRAW INTO GOLD</t>
+  </si>
+  <si>
+    <t>STRIKES TWICE</t>
+  </si>
+  <si>
+    <t>STRING &amp; KEY</t>
   </si>
   <si>
     <t>1Y</t>
   </si>
   <si>
-    <t>Sundown Orchid</t>
+    <t>SUNDOWN ORCHID</t>
   </si>
   <si>
     <t>SURF</t>
@@ -953,10 +952,10 @@
     <t>TEA PARTY</t>
   </si>
   <si>
-    <t>Tex mex</t>
-  </si>
-  <si>
-    <t>the king</t>
+    <t>TEX MEX</t>
+  </si>
+  <si>
+    <t>THE KING</t>
   </si>
   <si>
     <t>TIDAL</t>
@@ -965,52 +964,52 @@
     <t>TIDEWATER</t>
   </si>
   <si>
-    <t>tiffany box</t>
-  </si>
-  <si>
-    <t>Time Away</t>
-  </si>
-  <si>
-    <t>Tokyo Cream</t>
-  </si>
-  <si>
-    <t>Torchwood</t>
+    <t>TIFFANY BOX</t>
+  </si>
+  <si>
+    <t>TIME AWAY</t>
+  </si>
+  <si>
+    <t>TOKYO CREAM</t>
+  </si>
+  <si>
+    <t>TORCHWOOD</t>
   </si>
   <si>
     <t>TRANQUIL</t>
   </si>
   <si>
-    <t>true to life</t>
-  </si>
-  <si>
-    <t>Tucson</t>
-  </si>
-  <si>
-    <t>Tumbleweed</t>
-  </si>
-  <si>
-    <t>Tussie Mussie</t>
-  </si>
-  <si>
-    <t>Unimaginable</t>
-  </si>
-  <si>
-    <t>universe is Yours</t>
+    <t>TRUE TO LIFE</t>
+  </si>
+  <si>
+    <t>TUCSON</t>
+  </si>
+  <si>
+    <t>TUMBLEWEED</t>
+  </si>
+  <si>
+    <t>TUSSIE MUSSIE</t>
+  </si>
+  <si>
+    <t>UNIMAGINABLE</t>
+  </si>
+  <si>
+    <t>UNIVERSE IS YOURS</t>
   </si>
   <si>
     <t>4P</t>
   </si>
   <si>
-    <t>uptown electric</t>
-  </si>
-  <si>
-    <t>Urban fossil</t>
-  </si>
-  <si>
-    <t>Vague UNease</t>
-  </si>
-  <si>
-    <t>valentine</t>
+    <t>UPTOWN ELECTRIC</t>
+  </si>
+  <si>
+    <t>URBAN FOSSIL</t>
+  </si>
+  <si>
+    <t>VAGUE UNEASE</t>
+  </si>
+  <si>
+    <t>VALENTINE</t>
   </si>
   <si>
     <t>VELVET PORT</t>
@@ -1019,34 +1018,34 @@
     <t>VICTORIA</t>
   </si>
   <si>
-    <t>violet’s blueberry</t>
-  </si>
-  <si>
-    <t>visual purple</t>
+    <t>VIOLET’S BLUEBERRY</t>
+  </si>
+  <si>
+    <t>VISUAL PURPLE</t>
   </si>
   <si>
     <t>VIVID</t>
   </si>
   <si>
-    <t>watch my rising</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Way cool cristal </t>
-  </si>
-  <si>
-    <t>Whetstone</t>
-  </si>
-  <si>
-    <t>whip &amp; chill</t>
-  </si>
-  <si>
-    <t>whisper DOTS</t>
+    <t>WATCH MY RISING</t>
+  </si>
+  <si>
+    <t>WAY COOL CRISTAL</t>
+  </si>
+  <si>
+    <t>WHETSTONE</t>
+  </si>
+  <si>
+    <t>WHIP &amp; CHILL</t>
+  </si>
+  <si>
+    <t>WHISPER</t>
   </si>
   <si>
     <t>1B</t>
   </si>
   <si>
-    <t>Wicked Royal</t>
+    <t>WICKED ROYAL</t>
   </si>
   <si>
     <t>WILDERNESS</t>
@@ -1071,7 +1070,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -1083,7 +1082,7 @@
       <name val="Helvetica"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="13"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
     </font>
@@ -1130,12 +1129,6 @@
       <name val="Helvetica"/>
     </font>
     <font>
-      <b val="1"/>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Helvetica"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
@@ -1153,7 +1146,7 @@
       <name val="Helvetica"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1211,6 +1204,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="18"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="19"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -1439,11 +1438,11 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1473,15 +1472,6 @@
     <xf numFmtId="49" fontId="7" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1491,64 +1481,88 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="7" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="8" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="9" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="10" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="9" fillId="6" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="11" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="7" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="8" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="9" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="5" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="10" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1560,136 +1574,124 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="9" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="9" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="7" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="9" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="11" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="8" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="9" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="9" fillId="9" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="9" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="11" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="6" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="9" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="9" fillId="10" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="8" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="10" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="8" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="8" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="8" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="10" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="5" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="8" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="9" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1712,6 +1714,7 @@
       <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ff515151"/>
       <rgbColor rgb="ffffdd37"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffd5d5d5"/>
       <rgbColor rgb="ff75d5ff"/>
       <rgbColor rgb="ffeaeaea"/>
@@ -1735,10 +1738,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="404040"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="BFBFBF"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="499BC9"/>
@@ -1767,14 +1770,14 @@
     </a:clrScheme>
     <a:fontScheme name="Blank">
       <a:majorFont>
-        <a:latin typeface="Helvetica"/>
-        <a:ea typeface="Helvetica"/>
-        <a:cs typeface="Helvetica"/>
+        <a:latin typeface="Helvetica Neue"/>
+        <a:ea typeface="Helvetica Neue"/>
+        <a:cs typeface="Helvetica Neue"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Helvetica"/>
-        <a:ea typeface="Helvetica"/>
-        <a:cs typeface="Helvetica"/>
+        <a:latin typeface="Helvetica Neue"/>
+        <a:ea typeface="Helvetica Neue"/>
+        <a:cs typeface="Helvetica Neue"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Blank">
@@ -1932,14 +1935,15 @@
   <a:objectDefaults>
     <a:spDef>
       <a:spPr>
-        <a:blipFill rotWithShape="1">
-          <a:blip r:embed="rId1"/>
-          <a:srcRect l="0" t="0" r="0" b="0"/>
-          <a:tile tx="0" ty="0" sx="100000" sy="100000" flip="none" algn="tl"/>
-        </a:blipFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst>
           <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
@@ -1954,7 +1958,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1969,25 +1973,19 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
             <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
+              <a:srgbClr val="000000"/>
             </a:solidFill>
-            <a:effectLst>
-              <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="25400" dist="23998" dir="2700000">
-                <a:srgbClr val="000000">
-                  <a:alpha val="31034"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
             <a:uFillTx/>
             <a:latin typeface="+mn-lt"/>
             <a:ea typeface="+mn-ea"/>
             <a:cs typeface="+mn-cs"/>
-            <a:sym typeface="Helvetica"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -2235,14 +2233,20 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="6350" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
-        <a:effectLst/>
+        <a:effectLst>
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:srgbClr val="000000">
+              <a:alpha val="50000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -2531,7 +2535,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -2558,7 +2562,7 @@
             <a:latin typeface="+mn-lt"/>
             <a:ea typeface="+mn-ea"/>
             <a:cs typeface="+mn-cs"/>
-            <a:sym typeface="Helvetica"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -2811,20 +2815,18 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:AC277"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.73896" defaultRowHeight="16.3" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.66667" defaultRowHeight="16.3" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="22.1719" style="1" customWidth="1"/>
-    <col min="2" max="3" width="6.97656" style="1" customWidth="1"/>
-    <col min="4" max="5" width="15.8281" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.3125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.4609" style="1" customWidth="1"/>
-    <col min="8" max="9" width="12.3203" style="1" customWidth="1"/>
+    <col min="2" max="3" width="7" style="1" customWidth="1"/>
+    <col min="4" max="5" width="15.8516" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.3516" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5" style="1" customWidth="1"/>
+    <col min="8" max="9" width="12.3516" style="1" customWidth="1"/>
     <col min="10" max="29" width="18" style="1" customWidth="1"/>
-    <col min="30" max="256" width="9.75781" style="1" customWidth="1"/>
+    <col min="30" max="256" width="9.67188" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="43" customHeight="1">
@@ -4965,7 +4967,7 @@
       <c r="AC55" s="16"/>
     </row>
     <row r="56" ht="27" customHeight="1">
-      <c r="A56" t="s" s="10">
+      <c r="A56" t="s" s="50">
         <v>110</v>
       </c>
       <c r="B56" t="s" s="11">
@@ -5041,7 +5043,7 @@
       <c r="AC57" s="16"/>
     </row>
     <row r="58" ht="27" customHeight="1">
-      <c r="A58" t="s" s="50">
+      <c r="A58" t="s" s="51">
         <v>114</v>
       </c>
       <c r="B58" t="s" s="11">
@@ -5231,10 +5233,10 @@
       <c r="AC62" s="13"/>
     </row>
     <row r="63" ht="27" customHeight="1">
-      <c r="A63" t="s" s="51">
+      <c r="A63" t="s" s="52">
         <v>119</v>
       </c>
-      <c r="B63" s="52"/>
+      <c r="B63" s="53"/>
       <c r="C63" s="15">
         <f>SUM(D63:AC63)</f>
         <v>0</v>
@@ -5343,7 +5345,7 @@
       <c r="AC65" s="16"/>
     </row>
     <row r="66" ht="27" customHeight="1">
-      <c r="A66" t="s" s="50">
+      <c r="A66" t="s" s="51">
         <v>122</v>
       </c>
       <c r="B66" t="s" s="11">
@@ -5495,7 +5497,7 @@
       <c r="AC69" s="16"/>
     </row>
     <row r="70" ht="27" customHeight="1">
-      <c r="A70" t="s" s="10">
+      <c r="A70" t="s" s="54">
         <v>126</v>
       </c>
       <c r="B70" t="s" s="11">
@@ -5533,7 +5535,7 @@
       <c r="AC70" s="13"/>
     </row>
     <row r="71" ht="27" customHeight="1">
-      <c r="A71" t="s" s="53">
+      <c r="A71" t="s" s="55">
         <v>128</v>
       </c>
       <c r="B71" t="s" s="14">
@@ -5571,7 +5573,7 @@
       <c r="AC71" s="16"/>
     </row>
     <row r="72" ht="27" customHeight="1">
-      <c r="A72" t="s" s="53">
+      <c r="A72" t="s" s="55">
         <v>129</v>
       </c>
       <c r="B72" t="s" s="11">
@@ -5622,7 +5624,7 @@
       <c r="D73" s="16"/>
       <c r="E73" s="16"/>
       <c r="F73" s="16"/>
-      <c r="G73" s="54"/>
+      <c r="G73" s="56"/>
       <c r="H73" s="23"/>
       <c r="I73" s="24"/>
       <c r="J73" s="16"/>
@@ -5774,7 +5776,7 @@
       <c r="D77" s="28"/>
       <c r="E77" s="16"/>
       <c r="F77" s="16"/>
-      <c r="G77" s="54"/>
+      <c r="G77" s="56"/>
       <c r="H77" s="23"/>
       <c r="I77" s="24"/>
       <c r="J77" s="16"/>
@@ -5926,7 +5928,7 @@
       <c r="D81" s="16"/>
       <c r="E81" s="16"/>
       <c r="F81" s="16"/>
-      <c r="G81" s="54"/>
+      <c r="G81" s="56"/>
       <c r="H81" s="27"/>
       <c r="I81" s="28"/>
       <c r="J81" s="16"/>
@@ -6306,7 +6308,7 @@
       <c r="D91" s="28"/>
       <c r="E91" s="16"/>
       <c r="F91" s="16"/>
-      <c r="G91" s="54"/>
+      <c r="G91" s="56"/>
       <c r="H91" s="23"/>
       <c r="I91" s="24"/>
       <c r="J91" s="16"/>
@@ -6379,7 +6381,7 @@
         <f>SUM(D93:AC93)</f>
         <v>0</v>
       </c>
-      <c r="D93" s="55"/>
+      <c r="D93" s="57"/>
       <c r="E93" s="23"/>
       <c r="F93" s="23"/>
       <c r="G93" s="23"/>
@@ -6610,7 +6612,7 @@
       <c r="D99" s="16"/>
       <c r="E99" s="16"/>
       <c r="F99" s="16"/>
-      <c r="G99" s="54"/>
+      <c r="G99" s="56"/>
       <c r="H99" s="23"/>
       <c r="I99" s="24"/>
       <c r="J99" s="16"/>
@@ -6673,7 +6675,7 @@
       <c r="AC100" s="13"/>
     </row>
     <row r="101" ht="27" customHeight="1">
-      <c r="A101" t="s" s="56">
+      <c r="A101" t="s" s="58">
         <v>163</v>
       </c>
       <c r="B101" t="s" s="14">
@@ -6711,7 +6713,7 @@
       <c r="AC101" s="16"/>
     </row>
     <row r="102" ht="27" customHeight="1">
-      <c r="A102" t="s" s="50">
+      <c r="A102" t="s" s="51">
         <v>164</v>
       </c>
       <c r="B102" t="s" s="11">
@@ -6749,7 +6751,7 @@
       <c r="AC102" s="13"/>
     </row>
     <row r="103" ht="27" customHeight="1">
-      <c r="A103" t="s" s="53">
+      <c r="A103" t="s" s="55">
         <v>165</v>
       </c>
       <c r="B103" t="s" s="14">
@@ -6825,7 +6827,7 @@
       <c r="AC104" s="13"/>
     </row>
     <row r="105" ht="27" customHeight="1">
-      <c r="A105" t="s" s="53">
+      <c r="A105" t="s" s="55">
         <v>167</v>
       </c>
       <c r="B105" t="s" s="14">
@@ -6990,7 +6992,7 @@
       <c r="D109" s="16"/>
       <c r="E109" s="16"/>
       <c r="F109" s="16"/>
-      <c r="G109" s="54"/>
+      <c r="G109" s="56"/>
       <c r="H109" s="23"/>
       <c r="I109" s="24"/>
       <c r="J109" s="16"/>
@@ -7129,7 +7131,7 @@
       <c r="AC112" s="13"/>
     </row>
     <row r="113" ht="27" customHeight="1">
-      <c r="A113" t="s" s="50">
+      <c r="A113" t="s" s="51">
         <v>175</v>
       </c>
       <c r="B113" t="s" s="14">
@@ -7143,7 +7145,7 @@
       <c r="E113" s="27"/>
       <c r="F113" s="27"/>
       <c r="G113" s="27"/>
-      <c r="H113" s="57"/>
+      <c r="H113" s="59"/>
       <c r="I113" s="35"/>
       <c r="J113" s="16"/>
       <c r="K113" s="16"/>
@@ -7280,7 +7282,7 @@
       <c r="AB116" s="13"/>
       <c r="AC116" s="13"/>
     </row>
-    <row r="117" ht="36.65" customHeight="1">
+    <row r="117" ht="25.85" customHeight="1">
       <c r="A117" t="s" s="29">
         <v>179</v>
       </c>
@@ -7370,7 +7372,7 @@
       <c r="D119" s="16"/>
       <c r="E119" s="16"/>
       <c r="F119" s="16"/>
-      <c r="G119" s="54"/>
+      <c r="G119" s="56"/>
       <c r="H119" s="23"/>
       <c r="I119" s="24"/>
       <c r="J119" s="16"/>
@@ -7395,7 +7397,7 @@
       <c r="AC119" s="16"/>
     </row>
     <row r="120" ht="27" customHeight="1">
-      <c r="A120" t="s" s="53">
+      <c r="A120" t="s" s="55">
         <v>182</v>
       </c>
       <c r="B120" t="s" s="11">
@@ -7446,7 +7448,7 @@
       <c r="D121" s="16"/>
       <c r="E121" s="16"/>
       <c r="F121" s="16"/>
-      <c r="G121" s="54"/>
+      <c r="G121" s="56"/>
       <c r="H121" s="23"/>
       <c r="I121" s="24"/>
       <c r="J121" s="16"/>
@@ -7737,7 +7739,7 @@
       <c r="AC128" s="13"/>
     </row>
     <row r="129" ht="27" customHeight="1">
-      <c r="A129" t="s" s="53">
+      <c r="A129" t="s" s="55">
         <v>191</v>
       </c>
       <c r="B129" t="s" s="14">
@@ -7751,7 +7753,7 @@
       <c r="E129" s="36"/>
       <c r="F129" s="36"/>
       <c r="G129" s="37"/>
-      <c r="H129" s="57"/>
+      <c r="H129" s="59"/>
       <c r="I129" s="35"/>
       <c r="J129" s="16"/>
       <c r="K129" s="16"/>
@@ -7813,7 +7815,7 @@
       <c r="AC130" s="13"/>
     </row>
     <row r="131" ht="27" customHeight="1">
-      <c r="A131" t="s" s="58">
+      <c r="A131" t="s" s="60">
         <v>193</v>
       </c>
       <c r="B131" t="s" s="14">
@@ -7851,7 +7853,7 @@
       <c r="AC131" s="16"/>
     </row>
     <row r="132" ht="27" customHeight="1">
-      <c r="A132" t="s" s="59">
+      <c r="A132" t="s" s="61">
         <v>195</v>
       </c>
       <c r="B132" t="s" s="33">
@@ -7889,7 +7891,7 @@
       <c r="AC132" s="13"/>
     </row>
     <row r="133" ht="27" customHeight="1">
-      <c r="A133" t="s" s="60">
+      <c r="A133" t="s" s="62">
         <v>196</v>
       </c>
       <c r="B133" t="s" s="14">
@@ -8054,7 +8056,7 @@
       <c r="D137" s="28"/>
       <c r="E137" s="16"/>
       <c r="F137" s="16"/>
-      <c r="G137" s="54"/>
+      <c r="G137" s="56"/>
       <c r="H137" s="23"/>
       <c r="I137" s="24"/>
       <c r="J137" s="16"/>
@@ -8763,7 +8765,7 @@
       <c r="AC155" s="16"/>
     </row>
     <row r="156" ht="27" customHeight="1">
-      <c r="A156" t="s" s="50">
+      <c r="A156" t="s" s="51">
         <v>221</v>
       </c>
       <c r="B156" t="s" s="11">
@@ -8915,7 +8917,7 @@
       <c r="AC159" s="16"/>
     </row>
     <row r="160" ht="27" customHeight="1">
-      <c r="A160" t="s" s="50">
+      <c r="A160" t="s" s="51">
         <v>225</v>
       </c>
       <c r="B160" t="s" s="11">
@@ -8991,7 +8993,7 @@
       <c r="AC161" s="16"/>
     </row>
     <row r="162" ht="27" customHeight="1">
-      <c r="A162" t="s" s="53">
+      <c r="A162" t="s" s="55">
         <v>228</v>
       </c>
       <c r="B162" t="s" s="11">
@@ -9067,7 +9069,7 @@
       <c r="AC163" s="16"/>
     </row>
     <row r="164" ht="27" customHeight="1">
-      <c r="A164" t="s" s="50">
+      <c r="A164" t="s" s="51">
         <v>230</v>
       </c>
       <c r="B164" t="s" s="11">
@@ -9118,7 +9120,7 @@
       <c r="D165" s="28"/>
       <c r="E165" s="16"/>
       <c r="F165" s="16"/>
-      <c r="G165" s="54"/>
+      <c r="G165" s="56"/>
       <c r="H165" s="23"/>
       <c r="I165" s="24"/>
       <c r="J165" s="16"/>
@@ -9371,7 +9373,7 @@
       <c r="AC171" s="16"/>
     </row>
     <row r="172" ht="27" customHeight="1">
-      <c r="A172" t="s" s="53">
+      <c r="A172" t="s" s="55">
         <v>238</v>
       </c>
       <c r="B172" t="s" s="11">
@@ -9574,7 +9576,7 @@
       <c r="D177" s="16"/>
       <c r="E177" s="16"/>
       <c r="F177" s="16"/>
-      <c r="G177" s="54"/>
+      <c r="G177" s="56"/>
       <c r="H177" s="23"/>
       <c r="I177" s="24"/>
       <c r="J177" s="16"/>
@@ -9675,7 +9677,7 @@
       <c r="AC179" s="16"/>
     </row>
     <row r="180" ht="27" customHeight="1">
-      <c r="A180" t="s" s="56">
+      <c r="A180" t="s" s="58">
         <v>247</v>
       </c>
       <c r="B180" t="s" s="11">
@@ -10017,7 +10019,7 @@
       <c r="AC188" s="13"/>
     </row>
     <row r="189" ht="27" customHeight="1">
-      <c r="A189" t="s" s="56">
+      <c r="A189" t="s" s="58">
         <v>256</v>
       </c>
       <c r="B189" t="s" s="14">
@@ -10169,7 +10171,7 @@
       <c r="AC192" s="13"/>
     </row>
     <row r="193" ht="27" customHeight="1">
-      <c r="A193" t="s" s="56">
+      <c r="A193" t="s" s="58">
         <v>260</v>
       </c>
       <c r="B193" t="s" s="14">
@@ -10207,7 +10209,7 @@
       <c r="AC193" s="16"/>
     </row>
     <row r="194" ht="27" customHeight="1">
-      <c r="A194" t="s" s="56">
+      <c r="A194" t="s" s="58">
         <v>261</v>
       </c>
       <c r="B194" t="s" s="11">
@@ -10359,7 +10361,7 @@
       <c r="AC197" s="16"/>
     </row>
     <row r="198" ht="27" customHeight="1">
-      <c r="A198" t="s" s="50">
+      <c r="A198" t="s" s="51">
         <v>265</v>
       </c>
       <c r="B198" t="s" s="11">
@@ -10549,7 +10551,7 @@
       <c r="AC202" s="13"/>
     </row>
     <row r="203" ht="27" customHeight="1">
-      <c r="A203" t="s" s="10">
+      <c r="A203" t="s" s="50">
         <v>270</v>
       </c>
       <c r="B203" t="s" s="14">
@@ -10587,7 +10589,7 @@
       <c r="AC203" s="16"/>
     </row>
     <row r="204" ht="27" customHeight="1">
-      <c r="A204" t="s" s="53">
+      <c r="A204" t="s" s="55">
         <v>271</v>
       </c>
       <c r="B204" t="s" s="11">
@@ -10853,7 +10855,7 @@
       <c r="AC210" s="13"/>
     </row>
     <row r="211" ht="27" customHeight="1">
-      <c r="A211" t="s" s="61">
+      <c r="A211" t="s" s="63">
         <v>278</v>
       </c>
       <c r="B211" t="s" s="14">
@@ -10891,7 +10893,7 @@
       <c r="AC211" s="16"/>
     </row>
     <row r="212" ht="27" customHeight="1">
-      <c r="A212" t="s" s="62">
+      <c r="A212" t="s" s="64">
         <v>279</v>
       </c>
       <c r="B212" t="s" s="11">
@@ -11043,7 +11045,7 @@
       <c r="AC215" s="16"/>
     </row>
     <row r="216" ht="27" customHeight="1">
-      <c r="A216" t="s" s="10">
+      <c r="A216" t="s" s="54">
         <v>283</v>
       </c>
       <c r="B216" t="s" s="11">
@@ -11246,7 +11248,7 @@
       <c r="D221" s="28"/>
       <c r="E221" s="16"/>
       <c r="F221" s="16"/>
-      <c r="G221" s="54"/>
+      <c r="G221" s="56"/>
       <c r="H221" s="27"/>
       <c r="I221" s="28"/>
       <c r="J221" s="16"/>
@@ -11461,7 +11463,7 @@
       <c r="AC226" s="13"/>
     </row>
     <row r="227" ht="27" customHeight="1">
-      <c r="A227" t="s" s="53">
+      <c r="A227" t="s" s="55">
         <v>295</v>
       </c>
       <c r="B227" t="s" s="14">
@@ -11550,7 +11552,7 @@
       <c r="D229" s="28"/>
       <c r="E229" s="16"/>
       <c r="F229" s="16"/>
-      <c r="G229" s="54"/>
+      <c r="G229" s="56"/>
       <c r="H229" s="23"/>
       <c r="I229" s="24"/>
       <c r="J229" s="16"/>
@@ -11703,7 +11705,7 @@
       <c r="E233" s="27"/>
       <c r="F233" s="27"/>
       <c r="G233" s="27"/>
-      <c r="H233" s="57"/>
+      <c r="H233" s="59"/>
       <c r="I233" s="35"/>
       <c r="J233" s="16"/>
       <c r="K233" s="16"/>
@@ -11955,7 +11957,7 @@
       <c r="AC239" s="16"/>
     </row>
     <row r="240" ht="27" customHeight="1">
-      <c r="A240" t="s" s="50">
+      <c r="A240" t="s" s="51">
         <v>310</v>
       </c>
       <c r="B240" t="s" s="11">
@@ -12031,7 +12033,7 @@
       <c r="AC241" s="16"/>
     </row>
     <row r="242" ht="27" customHeight="1">
-      <c r="A242" t="s" s="63">
+      <c r="A242" t="s" s="65">
         <v>312</v>
       </c>
       <c r="B242" t="s" s="11">
@@ -12107,7 +12109,7 @@
       <c r="AC243" s="16"/>
     </row>
     <row r="244" ht="27" customHeight="1">
-      <c r="A244" t="s" s="51">
+      <c r="A244" t="s" s="52">
         <v>314</v>
       </c>
       <c r="B244" t="s" s="11">
@@ -12307,11 +12309,11 @@
         <f>SUM(D249:AC249)</f>
         <v>0</v>
       </c>
-      <c r="D249" s="57"/>
-      <c r="E249" s="57"/>
-      <c r="F249" s="57"/>
-      <c r="G249" s="57"/>
-      <c r="H249" s="57"/>
+      <c r="D249" s="59"/>
+      <c r="E249" s="59"/>
+      <c r="F249" s="59"/>
+      <c r="G249" s="59"/>
+      <c r="H249" s="59"/>
       <c r="I249" s="35"/>
       <c r="J249" s="16"/>
       <c r="K249" s="16"/>
@@ -12373,10 +12375,10 @@
       <c r="AC250" s="13"/>
     </row>
     <row r="251" ht="27" customHeight="1">
-      <c r="A251" t="s" s="64">
+      <c r="A251" t="s" s="29">
         <v>321</v>
       </c>
-      <c r="B251" t="s" s="65">
+      <c r="B251" t="s" s="66">
         <v>66</v>
       </c>
       <c r="C251" s="22">
@@ -12411,7 +12413,7 @@
       <c r="AC251" s="16"/>
     </row>
     <row r="252" ht="27" customHeight="1">
-      <c r="A252" t="s" s="63">
+      <c r="A252" t="s" s="65">
         <v>322</v>
       </c>
       <c r="B252" t="s" s="11">
@@ -12563,7 +12565,7 @@
       <c r="AC255" s="16"/>
     </row>
     <row r="256" ht="27" customHeight="1">
-      <c r="A256" t="s" s="63">
+      <c r="A256" t="s" s="65">
         <v>326</v>
       </c>
       <c r="B256" t="s" s="11">
@@ -12677,7 +12679,7 @@
       <c r="AC258" s="13"/>
     </row>
     <row r="259" ht="27" customHeight="1">
-      <c r="A259" t="s" s="51">
+      <c r="A259" t="s" s="52">
         <v>330</v>
       </c>
       <c r="B259" t="s" s="14">
@@ -12715,7 +12717,7 @@
       <c r="AC259" s="16"/>
     </row>
     <row r="260" ht="27" customHeight="1">
-      <c r="A260" t="s" s="66">
+      <c r="A260" t="s" s="67">
         <v>331</v>
       </c>
       <c r="B260" t="s" s="11">
@@ -12753,7 +12755,7 @@
       <c r="AC260" s="13"/>
     </row>
     <row r="261" ht="27" customHeight="1">
-      <c r="A261" t="s" s="63">
+      <c r="A261" t="s" s="65">
         <v>332</v>
       </c>
       <c r="B261" t="s" s="14">
@@ -12791,7 +12793,7 @@
       <c r="AC261" s="16"/>
     </row>
     <row r="262" ht="27" customHeight="1">
-      <c r="A262" t="s" s="63">
+      <c r="A262" t="s" s="65">
         <v>333</v>
       </c>
       <c r="B262" t="s" s="11">
@@ -12867,7 +12869,7 @@
       <c r="AC263" s="16"/>
     </row>
     <row r="264" ht="27" customHeight="1">
-      <c r="A264" t="s" s="63">
+      <c r="A264" t="s" s="65">
         <v>335</v>
       </c>
       <c r="B264" t="s" s="11">
@@ -13095,7 +13097,7 @@
       <c r="AC269" s="16"/>
     </row>
     <row r="270" ht="27" customHeight="1">
-      <c r="A270" t="s" s="51">
+      <c r="A270" t="s" s="52">
         <v>341</v>
       </c>
       <c r="B270" t="s" s="11">
@@ -13285,7 +13287,7 @@
       <c r="AC274" s="13"/>
     </row>
     <row r="275" ht="27" customHeight="1">
-      <c r="A275" t="s" s="63">
+      <c r="A275" t="s" s="65">
         <v>347</v>
       </c>
       <c r="B275" t="s" s="14">
@@ -13323,151 +13325,151 @@
       <c r="AC275" s="16"/>
     </row>
     <row r="276" ht="58.55" customHeight="1">
-      <c r="A276" t="s" s="67">
+      <c r="A276" t="s" s="68">
         <v>348</v>
       </c>
-      <c r="B276" s="68"/>
+      <c r="B276" s="69"/>
       <c r="C276" s="12">
         <f>SUM(D276:AC276)</f>
         <v>0</v>
       </c>
-      <c r="D276" s="69">
+      <c r="D276" s="70">
         <f>SUM(D2:D275)</f>
         <v>0</v>
       </c>
-      <c r="E276" s="69">
+      <c r="E276" s="70">
         <f>SUM(E2:E275)</f>
         <v>0</v>
       </c>
-      <c r="F276" s="69">
+      <c r="F276" s="70">
         <f>SUM(F2:F275)</f>
         <v>0</v>
       </c>
-      <c r="G276" s="70">
+      <c r="G276" s="71">
         <f>SUM(G2:G275)</f>
         <v>0</v>
       </c>
-      <c r="H276" s="71">
+      <c r="H276" s="72">
         <f>SUM(H2:H275)</f>
         <v>0</v>
       </c>
-      <c r="I276" s="72">
+      <c r="I276" s="73">
         <f>SUM(I2:I275)</f>
         <v>0</v>
       </c>
-      <c r="J276" s="69">
+      <c r="J276" s="70">
         <f>SUM(J2:J275)</f>
         <v>0</v>
       </c>
-      <c r="K276" s="69">
+      <c r="K276" s="70">
         <f>SUM(K2:K275)</f>
         <v>0</v>
       </c>
-      <c r="L276" s="69">
+      <c r="L276" s="70">
         <f>SUM(L2:L275)</f>
         <v>0</v>
       </c>
-      <c r="M276" s="69">
+      <c r="M276" s="70">
         <f>SUM(M2:M275)</f>
         <v>0</v>
       </c>
-      <c r="N276" s="69">
+      <c r="N276" s="70">
         <f>SUM(N2:N275)</f>
         <v>0</v>
       </c>
-      <c r="O276" s="69">
+      <c r="O276" s="70">
         <f>SUM(O2:O275)</f>
         <v>0</v>
       </c>
-      <c r="P276" s="69">
+      <c r="P276" s="70">
         <f>SUM(P2:P275)</f>
         <v>0</v>
       </c>
-      <c r="Q276" s="69">
+      <c r="Q276" s="70">
         <f>SUM(Q2:Q275)</f>
         <v>0</v>
       </c>
-      <c r="R276" s="69">
+      <c r="R276" s="70">
         <f>SUM(R2:R275)</f>
         <v>0</v>
       </c>
-      <c r="S276" s="69">
+      <c r="S276" s="70">
         <f>SUM(S2:S275)</f>
         <v>0</v>
       </c>
-      <c r="T276" s="69">
+      <c r="T276" s="70">
         <f>SUM(T2:T275)</f>
         <v>0</v>
       </c>
-      <c r="U276" s="69">
+      <c r="U276" s="70">
         <f>SUM(U2:U275)</f>
         <v>0</v>
       </c>
-      <c r="V276" s="69">
+      <c r="V276" s="70">
         <f>SUM(V2:V275)</f>
         <v>0</v>
       </c>
-      <c r="W276" s="69">
+      <c r="W276" s="70">
         <f>SUM(W2:W275)</f>
         <v>0</v>
       </c>
-      <c r="X276" s="69">
+      <c r="X276" s="70">
         <f>SUM(X2:X275)</f>
         <v>0</v>
       </c>
-      <c r="Y276" s="69">
+      <c r="Y276" s="70">
         <f>SUM(Y2:Y275)</f>
         <v>0</v>
       </c>
-      <c r="Z276" s="69">
+      <c r="Z276" s="70">
         <f>SUM(Z2:Z275)</f>
         <v>0</v>
       </c>
-      <c r="AA276" s="69">
+      <c r="AA276" s="70">
         <f>SUM(AA2:AA275)</f>
         <v>0</v>
       </c>
-      <c r="AB276" s="69">
+      <c r="AB276" s="70">
         <f>SUM(AB2:AB275)</f>
         <v>0</v>
       </c>
-      <c r="AC276" s="69">
+      <c r="AC276" s="70">
         <f>SUM(AC2:AC275)</f>
         <v>0</v>
       </c>
     </row>
     <row r="277" ht="58.55" customHeight="1">
-      <c r="A277" t="s" s="73">
+      <c r="A277" t="s" s="74">
         <v>349</v>
       </c>
-      <c r="B277" s="74"/>
-      <c r="C277" s="75"/>
-      <c r="D277" s="76"/>
-      <c r="E277" s="77"/>
-      <c r="F277" s="78"/>
-      <c r="G277" s="79"/>
-      <c r="H277" s="80"/>
-      <c r="I277" s="81"/>
-      <c r="J277" s="82"/>
-      <c r="K277" s="83"/>
-      <c r="L277" s="83"/>
-      <c r="M277" s="83"/>
-      <c r="N277" s="83"/>
-      <c r="O277" s="83"/>
-      <c r="P277" s="83"/>
-      <c r="Q277" s="83"/>
-      <c r="R277" s="83"/>
-      <c r="S277" s="83"/>
-      <c r="T277" s="83"/>
-      <c r="U277" s="83"/>
-      <c r="V277" s="83"/>
-      <c r="W277" s="83"/>
-      <c r="X277" s="83"/>
-      <c r="Y277" s="83"/>
-      <c r="Z277" s="83"/>
-      <c r="AA277" s="83"/>
-      <c r="AB277" s="83"/>
-      <c r="AC277" s="77"/>
+      <c r="B277" s="75"/>
+      <c r="C277" s="76"/>
+      <c r="D277" s="77"/>
+      <c r="E277" s="78"/>
+      <c r="F277" s="79"/>
+      <c r="G277" s="80"/>
+      <c r="H277" s="81"/>
+      <c r="I277" s="82"/>
+      <c r="J277" s="83"/>
+      <c r="K277" s="84"/>
+      <c r="L277" s="84"/>
+      <c r="M277" s="84"/>
+      <c r="N277" s="84"/>
+      <c r="O277" s="84"/>
+      <c r="P277" s="84"/>
+      <c r="Q277" s="84"/>
+      <c r="R277" s="84"/>
+      <c r="S277" s="84"/>
+      <c r="T277" s="84"/>
+      <c r="U277" s="84"/>
+      <c r="V277" s="84"/>
+      <c r="W277" s="84"/>
+      <c r="X277" s="84"/>
+      <c r="Y277" s="84"/>
+      <c r="Z277" s="84"/>
+      <c r="AA277" s="84"/>
+      <c r="AB277" s="84"/>
+      <c r="AC277" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>